<commit_message>
bubble chart for GO terms p-value/score/z-score
</commit_message>
<xml_diff>
--- a/gene_ontology_analysis/GO_results_compartments/compartment_go_analysis.xlsx
+++ b/gene_ontology_analysis/GO_results_compartments/compartment_go_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzakaya/Desktop/temporal gene/gene_ontology_analysis/GO_results_compartments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20CB53D0-0173-6B49-BD40-E29AD550487B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC777D2-5EC0-ED45-81FE-F7B5620DA830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29337,7 +29337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>

</xml_diff>